<commit_message>
committed day 2 and day 3 framework code
</commit_message>
<xml_diff>
--- a/Framework_SupportingExcel.xlsx
+++ b/Framework_SupportingExcel.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyTrainingWorkspace\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyTrainingWorkspace\mk-automation-framework-training\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47653470-3503-4D98-8F97-AECDBBD57C02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B36CD1C-241C-44E9-866D-8CC3D9A91167}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="560" activeTab="2" xr2:uid="{281D339B-0870-4E38-82E7-DD95B381E750}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="3" xr2:uid="{281D339B-0870-4E38-82E7-DD95B381E750}"/>
   </bookViews>
   <sheets>
     <sheet name="TDD Vs BDD" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="98">
   <si>
     <t>Cucumber</t>
   </si>
@@ -192,6 +193,144 @@
   </si>
   <si>
     <t>Create Feature files</t>
+  </si>
+  <si>
+    <t>Create Step Definitions</t>
+  </si>
+  <si>
+    <t>Paste code into Step Definitions</t>
+  </si>
+  <si>
+    <t>Run Feature file</t>
+  </si>
+  <si>
+    <t>Create hooks if necessory</t>
+  </si>
+  <si>
+    <t>Implement properties file</t>
+  </si>
+  <si>
+    <t>Create src/test/resources/conf/config.properties</t>
+  </si>
+  <si>
+    <t>Creating properties file</t>
+  </si>
+  <si>
+    <t>create a properties reader utility</t>
+  </si>
+  <si>
+    <t>Create PropertiesUtil class under src/test/util package</t>
+  </si>
+  <si>
+    <t>This method should read property file and load all properties into system propertes</t>
+  </si>
+  <si>
+    <t>In side your code, remove all hardcoded values and use properties</t>
+  </si>
+  <si>
+    <t>By using System.getProperty("propertyname")</t>
+  </si>
+  <si>
+    <t>Page Object Model / Page Factory</t>
+  </si>
+  <si>
+    <t>Its an approach or design pattern</t>
+  </si>
+  <si>
+    <t>We create one java class per page</t>
+  </si>
+  <si>
+    <t>That page contains all the webElements present in that particular page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">That page also contains the methods which act on those web elements </t>
+  </si>
+  <si>
+    <t xml:space="preserve">When you are creating a Java class for a web page: </t>
+  </si>
+  <si>
+    <t>Step 1 : Create a class with meaningful name</t>
+  </si>
+  <si>
+    <t>Step 2: Create a constructor inside the class which takes driver as parameter and initializes the page</t>
+  </si>
+  <si>
+    <t>Step 3: Create all web elements and provide locator using @FindBY/@FindAll</t>
+  </si>
+  <si>
+    <t>Step 4: Create methods which act on the web elements</t>
+  </si>
+  <si>
+    <t>Logging</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monitor,understand and debug your program execution </t>
+  </si>
+  <si>
+    <t>We are using log4j library for implementing logging in our framework</t>
+  </si>
+  <si>
+    <t>Add log4j dependency in pom.xml</t>
+  </si>
+  <si>
+    <t>log4j.xml</t>
+  </si>
+  <si>
+    <t>log4j library looks from log4j.xml in your project</t>
+  </si>
+  <si>
+    <t>log4j.xml contains while log4j configuration</t>
+  </si>
+  <si>
+    <t>Create log4j.xml file in your conf directory</t>
+  </si>
+  <si>
+    <t>Add conf directory to resources in your pom.xml</t>
+  </si>
+  <si>
+    <t>Create a logger object in each class</t>
+  </si>
+  <si>
+    <t>start logging</t>
+  </si>
+  <si>
+    <t>Data Driven Approach</t>
+  </si>
+  <si>
+    <t>What is data driven test?</t>
+  </si>
+  <si>
+    <t>Same test gets executed multiples times for different sets of test data</t>
+  </si>
+  <si>
+    <t>We use Scenario Outline in Cucumber</t>
+  </si>
+  <si>
+    <t>We use DataProvider in TestNG</t>
+  </si>
+  <si>
+    <t>fname</t>
+  </si>
+  <si>
+    <t>lname</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>Multiple ways of having test data</t>
+  </si>
+  <si>
+    <t>Directly in feature files Scenario Outline =&gt; Examples</t>
+  </si>
+  <si>
+    <t>For some tests, test data is sent from Excel files</t>
+  </si>
+  <si>
+    <t>user_number</t>
   </si>
 </sst>
 </file>
@@ -722,17 +861,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B26C46A-F037-418B-A725-4350F6B36078}">
-  <dimension ref="A3:F23"/>
+  <dimension ref="A3:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="47" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="71.453125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.7265625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -845,10 +984,1483 @@
         <v>51</v>
       </c>
     </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E25" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>4</v>
+      </c>
+      <c r="C29" t="s">
+        <v>56</v>
+      </c>
+      <c r="E29" t="s">
+        <v>58</v>
+      </c>
+      <c r="F29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E30" t="s">
+        <v>59</v>
+      </c>
+      <c r="F30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E32" t="s">
+        <v>62</v>
+      </c>
+      <c r="F32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>5</v>
+      </c>
+      <c r="C34" t="s">
+        <v>64</v>
+      </c>
+      <c r="E34" t="s">
+        <v>65</v>
+      </c>
+      <c r="F34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F36" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E38" t="s">
+        <v>69</v>
+      </c>
+      <c r="F38" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F39" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F40" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F41" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>6</v>
+      </c>
+      <c r="C43" t="s">
+        <v>74</v>
+      </c>
+      <c r="E43" t="s">
+        <v>75</v>
+      </c>
+      <c r="F43" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E44" t="s">
+        <v>77</v>
+      </c>
+      <c r="F44" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E45" t="s">
+        <v>79</v>
+      </c>
+      <c r="F45" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F46" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F47" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F48" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F49" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F50" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>7</v>
+      </c>
+      <c r="C52" t="s">
+        <v>86</v>
+      </c>
+      <c r="E52" t="s">
+        <v>87</v>
+      </c>
+      <c r="F52" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F53" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F54" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E56" t="s">
+        <v>94</v>
+      </c>
+      <c r="F56" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F57" t="s">
+        <v>96</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F15" r:id="rId1" xr:uid="{4432D7E9-249E-4A5B-AEF2-E31F804CE861}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85308FC7-BB6D-4916-A048-FC816F076245}">
+  <dimension ref="A1:AC237"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="M43" sqref="M43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L1" t="s">
+        <v>93</v>
+      </c>
+      <c r="M1" t="s">
+        <v>93</v>
+      </c>
+      <c r="N1" t="s">
+        <v>93</v>
+      </c>
+      <c r="O1" t="s">
+        <v>93</v>
+      </c>
+      <c r="P1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>93</v>
+      </c>
+      <c r="R1" t="s">
+        <v>93</v>
+      </c>
+      <c r="S1" t="s">
+        <v>93</v>
+      </c>
+      <c r="T1" t="s">
+        <v>93</v>
+      </c>
+      <c r="U1" t="s">
+        <v>93</v>
+      </c>
+      <c r="V1" t="s">
+        <v>93</v>
+      </c>
+      <c r="W1" t="s">
+        <v>93</v>
+      </c>
+      <c r="X1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A72">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A73">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A74">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A76">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A77">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A78">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A79">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A80">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A81">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A82">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A83">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A84">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A85">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A86">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A87">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A88">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A89">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A90">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A91">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A92">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A93">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A94">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A95">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A96">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A97">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A98">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A99">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A100">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A101">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A102">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A103">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A104">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A105">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A106">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A107">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A108">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A109">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A110">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A111">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A112">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A113">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A114">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A115">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A116">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A117">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A118">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A119">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A120">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A121">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A122">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A123">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A124">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A125">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A126">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A127">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A128">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A129">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A130">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A131">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A132">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A133">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A134">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A135">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A136">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A137">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A138">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A139">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A140">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A141">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A142">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A143">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A144">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A145">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A146">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A147">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A148">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A149">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A150">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A151">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A152">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A153">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A154">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A155">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A156">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A157">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A158">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A159">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A160">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A161">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A162">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A163">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A164">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A165">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A166">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A167">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A168">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A169">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A170">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A171">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A172">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A173">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A174">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A175">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A176">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A177">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A178">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A179">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A180">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A181">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A182">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A183">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A184">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A185">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A186">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A187">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A188">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A189">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A190">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A191">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A192">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A193">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A194">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A195">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A196">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A197">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A198">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A199">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A200">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A201">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A202">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A203">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A204">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A205">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A206">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A207">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A208">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A209">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A210">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A211">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A212">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A213">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A214">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A215">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A216">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A217">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A218">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A219">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A220">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A221">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A222">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A223">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A224">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A225">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A226">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A227">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A228">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A229">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A230">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A231">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A232">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A233">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A234">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A235">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A236">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A237">
+        <v>235</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>